<commit_message>
Update Tarefa de Stand Automóvel.xlsx
</commit_message>
<xml_diff>
--- a/files/Tarefa de Stand Automóvel.xlsx
+++ b/files/Tarefa de Stand Automóvel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaom\Documents\formacaotic.pt\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FFECC79-7F7E-42B0-9EDC-F4D3ABC500B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76551C2-06E1-4083-8469-0476FFAF2753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="592" xr2:uid="{DEB85460-7168-49A0-B261-E279683B372D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
   <si>
     <t>MODELO</t>
   </si>
@@ -252,18 +252,12 @@
     <t xml:space="preserve">Altere o nome da Folha1 para Automóveis Usados. </t>
   </si>
   <si>
-    <t>Destaque com a cor Verde (formatação condicional) todos os Tipos de Motor que sejam do tipo  elétrico</t>
-  </si>
-  <si>
     <t>Qual é a média dos Preço base superiores ao valor de 10000€?</t>
   </si>
   <si>
     <t>Destaque com a cor Verde (formatação condicional) na coluna "Preços Base" os 5 valores mais altos</t>
   </si>
   <si>
-    <t>Destaque com a cor Amarelo (formatação condicional) na coluna "Preços Base" os 7 valores mais baixos</t>
-  </si>
-  <si>
     <t>Quantos carros são de cor Branco?</t>
   </si>
   <si>
@@ -271,6 +265,15 @@
   </si>
   <si>
     <t>MZ B 2500 TD</t>
+  </si>
+  <si>
+    <t>Destaque com a cor Vermelho (formatação condicional) na coluna "Preços Base" os 7 valores mais baixos</t>
+  </si>
+  <si>
+    <t>Destaque com a cor Verde (formatação condicional) na coluna "Tipos de Motor" que sejam do tipo elétrico</t>
+  </si>
+  <si>
+    <t>Destaque com a cor Amarelo (formatação condicional) na coluna "Modelo" os carros da Marca Renault</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -501,6 +504,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -510,49 +548,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,12 +562,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -938,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91CC01C1-3528-4861-8BE7-3FDA6B536CC3}">
-  <dimension ref="B1:K29"/>
+  <dimension ref="B1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,44 +955,44 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="J2" s="26" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="J2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="27"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
@@ -1015,14 +1010,14 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="J4" s="22" t="s">
+      <c r="H4" s="5"/>
+      <c r="J4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="23"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
@@ -1043,11 +1038,11 @@
       <c r="G5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="J5" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="K5" s="23"/>
+      <c r="H5" s="5"/>
+      <c r="J5" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
@@ -1065,14 +1060,14 @@
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="J6" s="22" t="s">
+      <c r="H6" s="5"/>
+      <c r="J6" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
@@ -1090,14 +1085,14 @@
       <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="J7" s="22" t="s">
+      <c r="H7" s="5"/>
+      <c r="J7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="23"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
@@ -1115,14 +1110,14 @@
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="J8" s="22" t="s">
+      <c r="H8" s="5"/>
+      <c r="J8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="23"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
@@ -1140,14 +1135,14 @@
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="J9" s="22" t="s">
+      <c r="H9" s="5"/>
+      <c r="J9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="23"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
@@ -1168,11 +1163,11 @@
       <c r="G10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="J10" s="22" t="s">
+      <c r="H10" s="5"/>
+      <c r="J10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="23"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
@@ -1193,11 +1188,11 @@
       <c r="G11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="J11" s="22" t="s">
+      <c r="H11" s="5"/>
+      <c r="J11" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="23"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
@@ -1218,11 +1213,11 @@
       <c r="G12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="J12" s="22" t="s">
+      <c r="H12" s="5"/>
+      <c r="J12" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="K12" s="23"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
@@ -1240,12 +1235,12 @@
       <c r="F13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="J13" s="33" t="s">
-        <v>72</v>
+      <c r="H13" s="5"/>
+      <c r="J13" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="K13" s="5"/>
     </row>
@@ -1268,11 +1263,11 @@
       <c r="G14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="J14" s="24" t="s">
+      <c r="H14" s="5"/>
+      <c r="J14" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
@@ -1290,12 +1285,12 @@
       <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="30"/>
+      <c r="H15" s="5"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="28"/>
     </row>
     <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="4" t="s">
@@ -1316,9 +1311,9 @@
       <c r="G16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="31"/>
+      <c r="H16" s="5"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
@@ -1339,8 +1334,8 @@
       <c r="G17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="J17" s="20"/>
+      <c r="H17" s="5"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
@@ -1361,7 +1356,7 @@
       <c r="G18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
@@ -1382,11 +1377,11 @@
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="J19" s="15" t="s">
+      <c r="H19" s="5"/>
+      <c r="J19" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="K19" s="15"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
@@ -1404,14 +1399,14 @@
       <c r="F20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="J20" s="34" t="s">
+      <c r="H20" s="5"/>
+      <c r="J20" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="34"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
@@ -1429,12 +1424,12 @@
       <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
+      <c r="H21" s="5"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
@@ -1455,11 +1450,11 @@
       <c r="G22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="J22" s="34" t="s">
+      <c r="H22" s="5"/>
+      <c r="J22" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="K22" s="34"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="6" t="s">
@@ -1480,52 +1475,63 @@
       <c r="G23" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
+      <c r="H23" s="14"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J24" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="K24" s="34"/>
+      <c r="J24" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" s="21"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J26" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" s="34"/>
+      <c r="J26" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K26" s="21"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J28" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="K28" s="34"/>
+      <c r="J28" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="K28" s="21"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="J30" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K30" s="21"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
     <mergeCell ref="J2:K3"/>
     <mergeCell ref="J20:K21"/>
     <mergeCell ref="J22:K23"/>
     <mergeCell ref="J24:K25"/>
     <mergeCell ref="J26:K27"/>
-    <mergeCell ref="J28:K29"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="K14:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1630,7 +1636,7 @@
         <v>2000</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.35">
@@ -1677,7 +1683,7 @@
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1718,10 +1724,10 @@
       </c>
     </row>
     <row r="15" spans="3:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>